<commit_message>
Added abililty to hash the IP address
</commit_message>
<xml_diff>
--- a/extras/sample_form/get_ip_address_sample.xlsx
+++ b/extras/sample_form/get_ip_address_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\get_ip_address\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\get_ip_address\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DB905E-8AB9-433C-AAE8-958D7D8ACD28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF1833-1445-43F0-8E5E-AA1F37B96577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="help-choices" sheetId="5" r:id="rId5"/>
     <sheet name="help-settings" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="379">
   <si>
     <t>type</t>
   </si>
@@ -2970,19 +2970,32 @@
     <t>ip_test</t>
   </si>
   <si>
-    <t>Your IP Address is  ${ip_address}</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">This is collecting your IP address for statistical purposes </t>
-  </si>
-  <si>
     <t>Give it a few seconds and you'll move to the next field</t>
   </si>
   <si>
     <t>display_ip_address</t>
+  </si>
+  <si>
+    <t>hashed_ip_address</t>
+  </si>
+  <si>
+    <t>This is collecting your IP address for statistical purpose</t>
+  </si>
+  <si>
+    <t>Your IP Address is  ${ip_address}
+Your hashed IP Address is  ${hashed_ip_address}</t>
+  </si>
+  <si>
+    <t>custom-get_ip_address(hash="yes")</t>
+  </si>
+  <si>
+    <t>This is collecting your IP address for with hashing enabled for statistical purpose</t>
+  </si>
+  <si>
+    <t>Count to 5 and try again</t>
   </si>
 </sst>
 </file>
@@ -3325,7 +3338,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="169">
     <dxf>
       <fill>
         <patternFill>
@@ -4044,6 +4057,263 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAC090"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9CDE5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7E4BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4BD97"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB3A2C7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBFBFBF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCC1DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBF1DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCD5B5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4680,12 +4950,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -4928,164 +5198,325 @@
         <v>366</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>367</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="46.8">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="14.4" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>370</v>
+      <c r="B14" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576 B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="133" priority="361">
+  <conditionalFormatting sqref="F1:F12 B1:C12 I1:I12 I14:I1048576 B14:C1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="168" priority="431">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576 O1:O1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="132" priority="362">
+  <conditionalFormatting sqref="B1:C12 O1:O12 I1:I12 I14:I1048576 O14:O1048576 B14:C1048576">
+    <cfRule type="expression" dxfId="167" priority="432">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="131" priority="363">
+  <conditionalFormatting sqref="F1:F12 B1:D12 B14:D1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="166" priority="433">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="130" priority="364">
+  <conditionalFormatting sqref="G1:H12 B1:D12 B14:D1048576 G14:H1048576">
+    <cfRule type="expression" dxfId="165" priority="434">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="129" priority="365">
+  <conditionalFormatting sqref="G1:H12 B1:D12 B14:D1048576 G14:H1048576">
+    <cfRule type="expression" dxfId="164" priority="435">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="128" priority="366">
+  <conditionalFormatting sqref="F1:F12 B1:C12 B14:C1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="163" priority="436">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="127" priority="367">
+  <conditionalFormatting sqref="F1:F12 B1:B12 B14:B1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="162" priority="437">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="126" priority="368">
+  <conditionalFormatting sqref="B1:C12 B14:C1048576">
+    <cfRule type="expression" dxfId="161" priority="438">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="369">
+    <cfRule type="expression" dxfId="160" priority="439">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="370">
+    <cfRule type="expression" dxfId="159" priority="440">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="123" priority="371">
+  <conditionalFormatting sqref="B1:B12 N1:N12 N14:N1048576 B14:B1048576">
+    <cfRule type="expression" dxfId="158" priority="441">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="122" priority="372">
+  <conditionalFormatting sqref="F1:F12 B1:C12 B14:C1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="157" priority="442">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="121" priority="373">
+  <conditionalFormatting sqref="F1:F12 B1:C12 B14:C1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="156" priority="443">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="120" priority="374">
+  <conditionalFormatting sqref="B1:C12 B14:C1048576">
+    <cfRule type="expression" dxfId="155" priority="444">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="119" priority="375">
+  <conditionalFormatting sqref="A1:W12 A14:W1048576 L13">
+    <cfRule type="expression" dxfId="154" priority="445">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="376">
+    <cfRule type="expression" dxfId="153" priority="446">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="377">
+    <cfRule type="expression" dxfId="152" priority="447">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="378">
+    <cfRule type="expression" dxfId="151" priority="448">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="379">
+    <cfRule type="expression" dxfId="150" priority="449">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="380">
+    <cfRule type="expression" dxfId="149" priority="450">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="381">
+    <cfRule type="expression" dxfId="148" priority="451">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="382">
+    <cfRule type="expression" dxfId="147" priority="452">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="383">
+    <cfRule type="expression" dxfId="146" priority="453">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="384">
+    <cfRule type="expression" dxfId="145" priority="454">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="385">
+    <cfRule type="expression" dxfId="144" priority="455">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="386">
+    <cfRule type="expression" dxfId="143" priority="456">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="387">
+    <cfRule type="expression" dxfId="142" priority="457">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="388">
+    <cfRule type="expression" dxfId="141" priority="458">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="389">
+    <cfRule type="expression" dxfId="140" priority="459">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="390">
+    <cfRule type="expression" dxfId="139" priority="460">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="391">
+    <cfRule type="expression" dxfId="138" priority="461">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="392">
+    <cfRule type="expression" dxfId="137" priority="462">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="393">
+    <cfRule type="expression" dxfId="136" priority="463">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="394">
+  <conditionalFormatting sqref="B1:B12 B14:B1048576">
+    <cfRule type="expression" dxfId="135" priority="464">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="99" priority="395">
+  <conditionalFormatting sqref="F1:F12 B1:B12 B14:B1048576 F14:F1048576">
+    <cfRule type="expression" dxfId="134" priority="465">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13:C13 I13">
+    <cfRule type="expression" dxfId="133" priority="1">
+      <formula>$A13="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 O13 I13">
+    <cfRule type="expression" dxfId="132" priority="2">
+      <formula>$A13="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13:D13">
+    <cfRule type="expression" dxfId="131" priority="3">
+      <formula>$A13="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:H13 B13:D13">
+    <cfRule type="expression" dxfId="130" priority="4">
+      <formula>$A13="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:H13 B13:D13">
+    <cfRule type="expression" dxfId="129" priority="5">
+      <formula>$A13="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13:C13">
+    <cfRule type="expression" dxfId="128" priority="6">
+      <formula>OR(AND(LEFT($A13, 16)="select_multiple ", LEN($A13)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A13, 17)))), AND(LEFT($A13, 11)="select_one ", LEN($A13)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A13, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13">
+    <cfRule type="expression" dxfId="127" priority="7">
+      <formula>OR($A13="audio audit", $A13="text audit", $A13="speed violations count", $A13="speed violations list", $A13="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="126" priority="8">
+      <formula>$A13="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="9">
+      <formula>$A13="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="10">
+      <formula>OR($A13="geopoint", $A13="geoshape", $A13="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13 N13">
+    <cfRule type="expression" dxfId="123" priority="11">
+      <formula>OR($A13="calculate", $A13="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13:C13">
+    <cfRule type="expression" dxfId="122" priority="12">
+      <formula>OR($A13="date", $A13="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13:C13">
+    <cfRule type="expression" dxfId="121" priority="13">
+      <formula>$A13="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="120" priority="14">
+      <formula>OR($A13="audio", $A13="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:K13 M13:W13">
+    <cfRule type="expression" dxfId="119" priority="15">
+      <formula>OR(AND(LEFT($A13, 14)="sensor_stream ", LEN($A13)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A13, 15)))), AND(LEFT($A13, 17)="sensor_statistic ", LEN($A13)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A13, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="16">
+      <formula>$A13="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="17">
+      <formula>OR($A13="audio", $A13="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="18">
+      <formula>$A13="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="19">
+      <formula>OR($A13="date", $A13="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="20">
+      <formula>OR($A13="calculate", $A13="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="21">
+      <formula>$A13="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="22">
+      <formula>$A13="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="23">
+      <formula>OR($A13="geopoint", $A13="geoshape", $A13="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="24">
+      <formula>OR($A13="audio audit", $A13="text audit", $A13="speed violations count", $A13="speed violations list", $A13="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="25">
+      <formula>OR($A13="username", $A13="phonenumber", $A13="start", $A13="end", $A13="deviceid", $A13="subscriberid", $A13="simserial", $A13="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="26">
+      <formula>OR(AND(LEFT($A13, 16)="select_multiple ", LEN($A13)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A13, 17)))), AND(LEFT($A13, 11)="select_one ", LEN($A13)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A13, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="27">
+      <formula>$A13="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="28">
+      <formula>$A13="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="29">
+      <formula>$A13="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="30">
+      <formula>$A13="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="31">
+      <formula>$A13="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="32">
+      <formula>$A13="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="33">
+      <formula>$A13="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="expression" dxfId="100" priority="34">
+      <formula>$A13="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13">
+    <cfRule type="expression" dxfId="99" priority="35">
+      <formula>OR(AND(LEFT($A13, 14)="sensor_stream ", LEN($A13)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A13, 15)))), AND(LEFT($A13, 17)="sensor_statistic ", LEN($A13)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A13, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5208,7 +5639,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2004011505</v>
+        <v>2004062013</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>